<commit_message>
Addition of Negative cases in ArchiveAPIs
</commit_message>
<xml_diff>
--- a/src/test/java/ArchiveAPI/Data/ArchiveAPI_Data.xlsx
+++ b/src/test/java/ArchiveAPI/Data/ArchiveAPI_Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APIAutomation\Automation_OMSAPI\src\test\java\ArchiveAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34C6487-C63B-4017-A925-089637DD8510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3518F65-F1DC-43AE-89FD-531720187096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="357" firstSheet="1" activeTab="2" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="357" firstSheet="2" activeTab="4" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="ArchiveLogin" sheetId="14" r:id="rId1"/>
-    <sheet name="ArchiveOrder" sheetId="13" r:id="rId2"/>
-    <sheet name="ArchiveExecution" sheetId="15" r:id="rId3"/>
-    <sheet name="ArchiveAudittrail" sheetId="16" r:id="rId4"/>
+    <sheet name="ArchiveLoginNegative" sheetId="17" r:id="rId2"/>
+    <sheet name="ArchiveOrder" sheetId="13" r:id="rId3"/>
+    <sheet name="ArchiveExecution" sheetId="15" r:id="rId4"/>
+    <sheet name="ArchiveAudittrail" sheetId="16" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="172">
   <si>
     <t>Content_Type</t>
   </si>
@@ -99,9 +100,6 @@
   </si>
   <si>
     <t>LSL</t>
-  </si>
-  <si>
-    <t>ArchiveLogin_TC0001</t>
   </si>
   <si>
     <t>Username</t>
@@ -828,6 +826,228 @@
         "requireTotalCount": true
     }
 }</t>
+  </si>
+  <si>
+    <t>[errors, type, title, status, traceId]</t>
+  </si>
+  <si>
+    <t>{
+    "loadOptions": {
+        "filter": [  
+                "account25",
+                "=",
+                "10001"
+        ],
+        "skip": 0,
+        "take": 2000,
+        "isCountQuery": false,
+        "requireTotalCount": true
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "loadOptions": {
+        "filter": [  
+                "account",
+                "&lt;&gt;&lt;&gt;",
+                "10001"
+        ],
+        "skip": 0,
+        "take": 2000,
+        "isCountQuery": false,
+        "requireTotalCount": true
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "loadOptions": {
+        "filter": [  
+               [ "account",
+                "=",
+                "10001" ],
+          [ "account",
+                "=",
+                "10002" ]
+        ],
+        "skip": 0,
+        "take": 2000,
+        "isCountQuery": false,
+        "requireTotalCount": true
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "loadOptions": {
+        "filter": [  
+               [ "account",
+                "=",
+                "10001" ],
+          [ "account",
+                "=",
+                "10002" ]
+        ],
+        "skip": "abcd",
+        "take": 200,
+        "isCountQuery": false,
+        "requireTotalCount": true
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "loadOptions": {
+        "filter": [  
+               [ "account",
+                "=",
+                "10001" ],
+          [ "account",
+                "=",
+                "10002" ]
+        ],
+        "skip": 25,
+        "take": "abcd",
+        "isCountQuery": false,
+        "requireTotalCount": true
+    }
+}</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>Verify_Archive_Executions_API_Without_Filter_Value_TC0022</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Executions_API_With_Invalid_FilterName_TC0023</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Executions_API_With_Invalid_FilterOperator_TC0024</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Executions_API_With_Invalid_Skip_Value_TC0026</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Executions_API_With_Invalid_take_Value_TC0027</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Executions_API_Without_FilterBody_Value_TC0028</t>
+  </si>
+  <si>
+    <t>Verify_Archive_Orders_API_Without_Filter_Value_TC0022</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Orders_API_With_Invalid_Skip_Value_TC0026</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Orders_API_With_Invalid_take_Value_TC0027</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Orders_API_Without_FilterBody_Value_TC0028</t>
+  </si>
+  <si>
+    <t>Verify_Archive_Audittrails_API_Without_Filter_Value_TC0022</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Audittrails_API_With_Invalid_Skip_Value_TC0026</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Audittrails_API_With_Invalid_take_Value_TC0027</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Audittrails_API_Without_FilterBody_Value_TC0028</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Orders_API_Invalid_ContentType_Value_TC0029</t>
+  </si>
+  <si>
+    <t>[type, title, status, traceId]</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Executions_API_Invalid_ContentType_Value_TC0029</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Audittrails_API_Invalid_ContentType_Value_TC0029</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Orders_API_Invalid_Endpoint_Value_TC0030</t>
+  </si>
+  <si>
+    <t>/int/oms/archive/api/v1/Order/Filter</t>
+  </si>
+  <si>
+    <t>/int/oms/archive/api/v1/AuditTrail/Filter</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Audittrails_API_Invalid_Endpoint_Value_TC0030</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Executions_API_Invalid_Endpoint_Value_TC0030</t>
+  </si>
+  <si>
+    <t>ArchiveLogin_NegativeCase_Invalid_ClientID_TC0002</t>
+  </si>
+  <si>
+    <t>ArchiveLogin_With_Valid_Inputs_TC0001</t>
+  </si>
+  <si>
+    <t>ArchiveLogin_NegativeCase_Invalid_ClientSecret_TC0003</t>
+  </si>
+  <si>
+    <t>ArchiveLogin_NegativeCase_Invalid_Username_TC0004</t>
+  </si>
+  <si>
+    <t>ArchiveLogin_NegativeCase_Invalid_BoothID_TC0005</t>
+  </si>
+  <si>
+    <t>c2m123456</t>
+  </si>
+  <si>
+    <t>secret123abcdfgh</t>
+  </si>
+  <si>
+    <t>qatest2712345</t>
+  </si>
+  <si>
+    <t>LSL12345</t>
+  </si>
+  <si>
+    <t>Error_Message</t>
+  </si>
+  <si>
+    <t>invalid_client</t>
+  </si>
+  <si>
+    <t>Invalid username or booth_id.</t>
+  </si>
+  <si>
+    <t>[accessToken, expiresIn, tokenType, refreshToken, scope, error, errorDescription, errorText]</t>
+  </si>
+  <si>
+    <t>Verify_Archive_Orders_API_Without_Operator_Filters_Combinations_TC0023</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Orders_API_With_Invalid_FilterName_TC0024</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Orders_API_With_Invalid_FilterOperator_TC0025</t>
+  </si>
+  <si>
+    <t>Verify_Archive_Executions_API_Without_Operator_Filters_Combinations_TC0023</t>
+  </si>
+  <si>
+    <t>/int/oms/archive/api/v1/Execution/Filter</t>
+  </si>
+  <si>
+    <t>Verify_Archive_Audittrails_API_Without_Operator_Filters_Combinations_TC0023</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Audittrails_API_With_Invalid_FilterName_TC0024</t>
+  </si>
+  <si>
+    <t>Verify_NegativeCase_Archive_Audittrails_API_With_Invalid_FilterOperator_TC0025</t>
   </si>
 </sst>
 </file>
@@ -905,7 +1125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -922,10 +1142,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1240,30 +1459,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E338EA-CE9F-4D41-9ED1-5720F4BE28E7}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:H2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="81.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1275,21 +1495,24 @@
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>15</v>
@@ -1308,6 +1531,9 @@
       </c>
       <c r="H2" s="5">
         <v>200</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1316,11 +1542,198 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7CCEFE-F88D-4019-AFAD-6D4207875F7A}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" customWidth="1"/>
+    <col min="10" max="10" width="81.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="5">
+        <v>400</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="5">
+        <v>400</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="5">
+        <v>400</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="5">
+        <v>400</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D56E2-D9E9-47B4-91F3-26434E16CD4C}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,10 +1772,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -1372,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="8">
         <v>200</v>
@@ -1382,10 +1795,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -1395,20 +1808,20 @@
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="8">
+        <v>200</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="8">
-        <v>200</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1418,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="8">
         <v>200</v>
@@ -1428,10 +1841,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1441,7 +1854,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="8">
         <v>200</v>
@@ -1451,10 +1864,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1464,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="8">
         <v>200</v>
@@ -1474,10 +1887,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1487,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" s="8">
         <v>200</v>
@@ -1497,10 +1910,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1510,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="8">
         <v>200</v>
@@ -1520,10 +1933,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1533,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="8">
         <v>200</v>
@@ -1543,10 +1956,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1556,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="8">
         <v>200</v>
@@ -1566,10 +1979,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -1579,7 +1992,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="8">
         <v>200</v>
@@ -1589,10 +2002,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -1602,7 +2015,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="8">
         <v>200</v>
@@ -1612,10 +2025,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1625,20 +2038,20 @@
         <v>1</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="8">
         <v>200</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1648,20 +2061,20 @@
         <v>1</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="8">
         <v>200</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1671,7 +2084,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15" s="8">
         <v>200</v>
@@ -1681,10 +2094,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -1694,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F16" s="8">
         <v>200</v>
@@ -1704,10 +2117,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -1717,7 +2130,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F17" s="8">
         <v>200</v>
@@ -1727,10 +2140,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="13" t="s">
+      <c r="A18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1740,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18" s="8">
         <v>200</v>
@@ -1750,10 +2163,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -1763,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="8">
         <v>200</v>
@@ -1773,10 +2186,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1786,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="8">
         <v>200</v>
@@ -1796,10 +2209,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="13" t="s">
+      <c r="A21" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -1809,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" s="8">
         <v>200</v>
@@ -1819,10 +2232,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1832,7 +2245,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F22" s="8">
         <v>200</v>
@@ -1840,6 +2253,207 @@
       <c r="G22" s="7" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="8">
+        <v>200</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="8">
+        <v>200</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="8">
+        <v>400</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="8">
+        <v>400</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F27" s="8">
+        <v>400</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="8">
+        <v>400</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8">
+        <v>400</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="8">
+        <v>415</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="8">
+        <v>404</v>
+      </c>
+      <c r="G31" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1848,64 +2462,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D330E7-9686-41B7-8243-079FED9B19D8}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="106.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>27</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="8">
         <v>200</v>
@@ -1915,21 +2529,21 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="F3" s="8">
         <v>200</v>
       </c>
@@ -1938,441 +2552,642 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="8">
+        <v>200</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="8">
-        <v>200</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="F5" s="8">
+        <v>200</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="8">
-        <v>200</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="F6" s="8">
+        <v>200</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="8">
-        <v>200</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="F7" s="8">
+        <v>200</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="B8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="8">
+        <v>200</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="8">
+        <v>200</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="8">
-        <v>200</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="8">
-        <v>200</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="9" t="s">
+      <c r="F10" s="8">
+        <v>200</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="8">
+        <v>200</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="8">
+        <v>200</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="8">
+        <v>200</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="8">
+        <v>200</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="8">
-        <v>200</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="8">
-        <v>200</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="8">
-        <v>200</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="F15" s="8">
+        <v>200</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="8">
+        <v>200</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="8">
+        <v>200</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="8">
+        <v>200</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="8">
+        <v>200</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="8">
+        <v>200</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="8">
+        <v>200</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="8">
+        <v>200</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="8">
+        <v>200</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="8">
+        <v>200</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="8">
+        <v>400</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F12" s="8">
-        <v>200</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="8">
-        <v>200</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="8">
-        <v>200</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="8">
-        <v>200</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="F16" s="8">
-        <v>200</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F17" s="8">
-        <v>200</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="8">
-        <v>200</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="8">
-        <v>200</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="8">
-        <v>200</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="8">
-        <v>200</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="8">
-        <v>200</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="8">
+        <v>400</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F27" s="8">
+        <v>400</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="8">
+        <v>400</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8">
+        <v>400</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="8">
+        <v>415</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="8">
+        <v>404</v>
+      </c>
+      <c r="G31" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2380,12 +3195,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD535BD-FCEF-4C7D-A395-D646E8440B4F}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,43 +3217,43 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="F2" s="8">
         <v>200</v>
       </c>
@@ -2447,20 +3262,20 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="8">
         <v>200</v>
@@ -2470,441 +3285,642 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="8">
+        <v>200</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="8">
-        <v>200</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="F5" s="8">
+        <v>200</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="8">
-        <v>200</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="F6" s="8">
+        <v>200</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="8">
-        <v>200</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="F7" s="8">
+        <v>200</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="B8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="8">
+        <v>200</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="8">
+        <v>200</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="8">
-        <v>200</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="8">
-        <v>200</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="9" t="s">
+      <c r="F10" s="8">
+        <v>200</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="8">
+        <v>200</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="8">
+        <v>200</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="8">
+        <v>200</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="8">
+        <v>200</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="8">
-        <v>200</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="8">
-        <v>200</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="8">
-        <v>200</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="8">
-        <v>200</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="8">
-        <v>200</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="F15" s="8">
+        <v>200</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="8">
+        <v>200</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="8">
-        <v>200</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="8">
-        <v>200</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="F16" s="8">
-        <v>200</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="F17" s="8">
+        <v>200</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F17" s="8">
-        <v>200</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="B18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="8">
+        <v>200</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="9" t="s">
+      <c r="B19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="8">
-        <v>200</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="F19" s="8">
+        <v>200</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="9" t="s">
+      <c r="B20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="8">
-        <v>200</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="F20" s="8">
+        <v>200</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="B21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="8">
-        <v>200</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="F21" s="8">
+        <v>200</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="9" t="s">
+      <c r="B22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="8">
-        <v>200</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="F22" s="8">
+        <v>200</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="8">
+        <v>200</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="8">
-        <v>200</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="8">
+        <v>200</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="8">
+        <v>400</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="8">
+        <v>400</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F27" s="8">
+        <v>400</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="8">
+        <v>400</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8">
+        <v>400</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="8">
+        <v>415</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="8">
+        <v>404</v>
+      </c>
+      <c r="G31" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactoring New changes Archive and MKT endpoints
</commit_message>
<xml_diff>
--- a/src/test/java/ArchiveAPI/Data/ArchiveAPI_Data.xlsx
+++ b/src/test/java/ArchiveAPI/Data/ArchiveAPI_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APIAutomation\Automation_OMSAPI\src\test\java\ArchiveAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3518F65-F1DC-43AE-89FD-531720187096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD09BA5-2036-4855-84D3-35F1307F34DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="357" firstSheet="2" activeTab="4" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="357" firstSheet="2" activeTab="4" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="ArchiveLogin" sheetId="14" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="162">
   <si>
     <t>Content_Type</t>
   </si>
@@ -960,33 +960,6 @@
     <t>Verify_NegativeCase_Archive_Audittrails_API_Without_FilterBody_Value_TC0028</t>
   </si>
   <si>
-    <t>Verify_NegativeCase_Archive_Orders_API_Invalid_ContentType_Value_TC0029</t>
-  </si>
-  <si>
-    <t>[type, title, status, traceId]</t>
-  </si>
-  <si>
-    <t>Verify_NegativeCase_Archive_Executions_API_Invalid_ContentType_Value_TC0029</t>
-  </si>
-  <si>
-    <t>Verify_NegativeCase_Archive_Audittrails_API_Invalid_ContentType_Value_TC0029</t>
-  </si>
-  <si>
-    <t>Verify_NegativeCase_Archive_Orders_API_Invalid_Endpoint_Value_TC0030</t>
-  </si>
-  <si>
-    <t>/int/oms/archive/api/v1/Order/Filter</t>
-  </si>
-  <si>
-    <t>/int/oms/archive/api/v1/AuditTrail/Filter</t>
-  </si>
-  <si>
-    <t>Verify_NegativeCase_Archive_Audittrails_API_Invalid_Endpoint_Value_TC0030</t>
-  </si>
-  <si>
-    <t>Verify_NegativeCase_Archive_Executions_API_Invalid_Endpoint_Value_TC0030</t>
-  </si>
-  <si>
     <t>ArchiveLogin_NegativeCase_Invalid_ClientID_TC0002</t>
   </si>
   <si>
@@ -1023,9 +996,6 @@
     <t>Invalid username or booth_id.</t>
   </si>
   <si>
-    <t>[accessToken, expiresIn, tokenType, refreshToken, scope, error, errorDescription, errorText]</t>
-  </si>
-  <si>
     <t>Verify_Archive_Orders_API_Without_Operator_Filters_Combinations_TC0023</t>
   </si>
   <si>
@@ -1038,9 +1008,6 @@
     <t>Verify_Archive_Executions_API_Without_Operator_Filters_Combinations_TC0023</t>
   </si>
   <si>
-    <t>/int/oms/archive/api/v1/Execution/Filter</t>
-  </si>
-  <si>
     <t>Verify_Archive_Audittrails_API_Without_Operator_Filters_Combinations_TC0023</t>
   </si>
   <si>
@@ -1048,6 +1015,9 @@
   </si>
   <si>
     <t>Verify_NegativeCase_Archive_Audittrails_API_With_Invalid_FilterOperator_TC0025</t>
+  </si>
+  <si>
+    <t>[access_token, expires_in, token_type, refresh_token, scope, error, error_description, errorText]</t>
   </si>
 </sst>
 </file>
@@ -1461,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E338EA-CE9F-4D41-9ED1-5720F4BE28E7}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,7 +1479,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>22</v>
@@ -1533,7 +1503,7 @@
         <v>200</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1546,7 +1516,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,7 +1530,7 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.42578125" customWidth="1"/>
-    <col min="10" max="10" width="81.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="89.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1589,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>10</v>
@@ -1597,7 +1567,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>22</v>
@@ -1606,7 +1576,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>16</v>
@@ -1621,15 +1591,15 @@
         <v>400</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>22</v>
@@ -1641,7 +1611,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>2</v>
@@ -1653,15 +1623,15 @@
         <v>400</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>22</v>
@@ -1676,7 +1646,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>19</v>
@@ -1685,15 +1655,15 @@
         <v>400</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>22</v>
@@ -1711,16 +1681,16 @@
         <v>2</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H5" s="5">
         <v>400</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1730,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D56E2-D9E9-47B4-91F3-26434E16CD4C}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,7 +1711,7 @@
     <col min="1" max="1" width="102.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="255.5703125" style="6" customWidth="1"/>
     <col min="6" max="6" width="32.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="6" bestFit="1" customWidth="1"/>
@@ -2279,7 +2249,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>3</v>
@@ -2302,7 +2272,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>3</v>
@@ -2325,7 +2295,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>3</v>
@@ -2412,48 +2382,6 @@
       <c r="G29" s="7" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="8">
-        <v>415</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="8">
-        <v>404</v>
-      </c>
-      <c r="G31" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2464,10 +2392,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D330E7-9686-41B7-8243-079FED9B19D8}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3013,7 +2941,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>3</v>
@@ -3146,48 +3074,6 @@
       <c r="G29" s="7" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="8">
-        <v>415</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="8">
-        <v>404</v>
-      </c>
-      <c r="G31" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3197,10 +3083,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD535BD-FCEF-4C7D-A395-D646E8440B4F}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3746,7 +3632,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>3</v>
@@ -3769,7 +3655,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>3</v>
@@ -3792,7 +3678,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>3</v>
@@ -3879,48 +3765,6 @@
       <c r="G29" s="7" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="8">
-        <v>415</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="8">
-        <v>404</v>
-      </c>
-      <c r="G31" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Archive Login Response changes
</commit_message>
<xml_diff>
--- a/src/test/java/ArchiveAPI/Data/ArchiveAPI_Data.xlsx
+++ b/src/test/java/ArchiveAPI/Data/ArchiveAPI_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APIAutomation\Automation_OMSAPI\src\test\java\ArchiveAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD09BA5-2036-4855-84D3-35F1307F34DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE90F8B-C610-4DE6-9B42-0133EB45615C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="357" firstSheet="2" activeTab="4" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="357" activeTab="1" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="ArchiveLogin" sheetId="14" r:id="rId1"/>
@@ -1017,7 +1017,7 @@
     <t>Verify_NegativeCase_Archive_Audittrails_API_With_Invalid_FilterOperator_TC0025</t>
   </si>
   <si>
-    <t>[access_token, expires_in, token_type, refresh_token, scope, error, error_description, errorText]</t>
+    <t>[accessToken, expiresIn, tokenType, refreshToken, scope, error, errorDescription, errorText]</t>
   </si>
 </sst>
 </file>
@@ -1432,7 +1432,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,7 +1445,7 @@
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="81.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="85" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1515,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7CCEFE-F88D-4019-AFAD-6D4207875F7A}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3085,7 +3085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD535BD-FCEF-4C7D-A395-D646E8440B4F}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>

</xml_diff>